<commit_message>
still trying to get Commonwealth working in timeseries
</commit_message>
<xml_diff>
--- a/03_OpenDSS_Circuits/Commonwealth_Circuit_Opendss/Loads_Text.xlsx
+++ b/03_OpenDSS_Circuits/Commonwealth_Circuit_Opendss/Loads_Text.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Loads_NCSU" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -2657,8 +2660,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2956,7 +2987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I359"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A339" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E363" sqref="E363"/>
     </sheetView>
   </sheetViews>

</xml_diff>